<commit_message>
added language change func
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -28,22 +28,28 @@
     <t>interest</t>
   </si>
   <si>
+    <t>language</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
     <t>Smith</t>
   </si>
   <si>
-    <t>vndciiwao@emltmp.com</t>
+    <t>taotylwao@emltmp.com</t>
   </si>
   <si>
     <t>meditation</t>
   </si>
   <si>
+    <t>en</t>
+  </si>
+  <si>
     <t>Marry</t>
   </si>
   <si>
-    <t>gxvttfcsn@emlpro.com</t>
+    <t>pshcamwao@emltmp.com</t>
   </si>
   <si>
     <t>nasa</t>
@@ -55,7 +61,7 @@
     <t>Kann</t>
   </si>
   <si>
-    <t>eonihewao@emltmp.com</t>
+    <t>ejkgnwcsn@emlpro.com</t>
   </si>
   <si>
     <t>Max</t>
@@ -67,7 +73,10 @@
     <t>olegimbarig@gmail.com</t>
   </si>
   <si>
-    <t>pet</t>
+    <t>тварини</t>
+  </si>
+  <si>
+    <t>ua</t>
   </si>
   <si>
     <t xml:space="preserve">Max </t>
@@ -76,7 +85,10 @@
     <t>maxyanish9@gmail.com</t>
   </si>
   <si>
-    <t>phone</t>
+    <t>hamster</t>
+  </si>
+  <si>
+    <t>de</t>
   </si>
 </sst>
 </file>
@@ -782,82 +794,94 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A3" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A4" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A5" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A6" s="14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A7" s="14"/>

</xml_diff>